<commit_message>
looked at solution for 88 and drafted implementation concept
</commit_message>
<xml_diff>
--- a/88. Merge Sorted Array/Whiteboards/Solution.xlsx
+++ b/88. Merge Sorted Array/Whiteboards/Solution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\88. Merge Sorted Array\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D951F1-1B9F-46D5-9B02-7A3529CBDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="14">
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>j+=1</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>SWAP</t>
+  </si>
+  <si>
+    <t>SWAPEND</t>
+  </si>
+  <si>
+    <t>i+=1</t>
+  </si>
+  <si>
+    <t>nums2</t>
+  </si>
+  <si>
+    <t>nums1</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,12 +92,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,10 +118,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,17 +443,930 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="N13:AJ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD88" sqref="AD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.7109375" style="1"/>
+    <col min="1" max="31" width="4.7109375" style="1"/>
+    <col min="32" max="32" width="4.7109375" style="3"/>
+    <col min="33" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="13" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>7</v>
+      </c>
+      <c r="T15" s="1">
+        <v>1</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2</v>
+      </c>
+      <c r="V15" s="1">
+        <v>3</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="1">
+        <v>2</v>
+      </c>
+      <c r="P18" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>7</v>
+      </c>
+      <c r="T18" s="1">
+        <v>1</v>
+      </c>
+      <c r="U18" s="1">
+        <v>2</v>
+      </c>
+      <c r="V18" s="1">
+        <v>3</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>7</v>
+      </c>
+      <c r="T21" s="1">
+        <v>1</v>
+      </c>
+      <c r="U21" s="1">
+        <v>2</v>
+      </c>
+      <c r="V21" s="2">
+        <v>3</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24" s="2">
+        <v>3</v>
+      </c>
+      <c r="P24" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>7</v>
+      </c>
+      <c r="T24" s="1">
+        <v>1</v>
+      </c>
+      <c r="U24" s="1">
+        <v>2</v>
+      </c>
+      <c r="V24" s="2">
+        <v>2</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="1">
+        <v>3</v>
+      </c>
+      <c r="P28" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>7</v>
+      </c>
+      <c r="T28" s="1">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1">
+        <v>2</v>
+      </c>
+      <c r="V28" s="1">
+        <v>2</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+      <c r="X28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="15:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O31" s="1">
+        <v>3</v>
+      </c>
+      <c r="P31" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>7</v>
+      </c>
+      <c r="T31" s="1">
+        <v>1</v>
+      </c>
+      <c r="U31" s="1">
+        <v>2</v>
+      </c>
+      <c r="V31" s="1">
+        <v>2</v>
+      </c>
+      <c r="W31" s="1">
+        <v>0</v>
+      </c>
+      <c r="X31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O34" s="1">
+        <v>3</v>
+      </c>
+      <c r="P34" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>7</v>
+      </c>
+      <c r="T34" s="1">
+        <v>1</v>
+      </c>
+      <c r="U34" s="1">
+        <v>2</v>
+      </c>
+      <c r="V34" s="1">
+        <v>2</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0</v>
+      </c>
+      <c r="X34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O37" s="1">
+        <v>3</v>
+      </c>
+      <c r="P37" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>7</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="U37" s="1">
+        <v>2</v>
+      </c>
+      <c r="V37" s="1">
+        <v>2</v>
+      </c>
+      <c r="W37" s="1">
+        <v>0</v>
+      </c>
+      <c r="X37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>7</v>
+      </c>
+      <c r="T44" s="1">
+        <v>2</v>
+      </c>
+      <c r="U44" s="1">
+        <v>4</v>
+      </c>
+      <c r="V44" s="1">
+        <v>8</v>
+      </c>
+      <c r="W44" s="1">
+        <v>0</v>
+      </c>
+      <c r="X44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF44" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="15:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O47" s="1">
+        <v>2</v>
+      </c>
+      <c r="P47" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>7</v>
+      </c>
+      <c r="T47" s="1">
+        <v>1</v>
+      </c>
+      <c r="U47" s="1">
+        <v>4</v>
+      </c>
+      <c r="V47" s="1">
+        <v>8</v>
+      </c>
+      <c r="W47" s="1">
+        <v>0</v>
+      </c>
+      <c r="X47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O50" s="1">
+        <v>4</v>
+      </c>
+      <c r="P50" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>7</v>
+      </c>
+      <c r="T50" s="1">
+        <v>1</v>
+      </c>
+      <c r="U50" s="1">
+        <v>2</v>
+      </c>
+      <c r="V50" s="1">
+        <v>8</v>
+      </c>
+      <c r="W50" s="1">
+        <v>0</v>
+      </c>
+      <c r="X50" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O53" s="1">
+        <v>4</v>
+      </c>
+      <c r="P53" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>7</v>
+      </c>
+      <c r="T53" s="1">
+        <v>1</v>
+      </c>
+      <c r="U53" s="1">
+        <v>2</v>
+      </c>
+      <c r="V53" s="1">
+        <v>8</v>
+      </c>
+      <c r="W53" s="1">
+        <v>0</v>
+      </c>
+      <c r="X53" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O57" s="1">
+        <v>8</v>
+      </c>
+      <c r="P57" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>7</v>
+      </c>
+      <c r="T57" s="1">
+        <v>1</v>
+      </c>
+      <c r="U57" s="1">
+        <v>2</v>
+      </c>
+      <c r="V57" s="1">
+        <v>4</v>
+      </c>
+      <c r="W57" s="1">
+        <v>0</v>
+      </c>
+      <c r="X57" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="15:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O60" s="1">
+        <v>8</v>
+      </c>
+      <c r="P60" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>7</v>
+      </c>
+      <c r="T60" s="1">
+        <v>1</v>
+      </c>
+      <c r="U60" s="1">
+        <v>2</v>
+      </c>
+      <c r="V60" s="1">
+        <v>4</v>
+      </c>
+      <c r="W60" s="1">
+        <v>0</v>
+      </c>
+      <c r="X60" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W81" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N82" s="1">
+        <v>-2</v>
+      </c>
+      <c r="O82" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82" s="1">
+        <v>1</v>
+      </c>
+      <c r="S82" s="1">
+        <v>0</v>
+      </c>
+      <c r="T82" s="1">
+        <v>0</v>
+      </c>
+      <c r="U82" s="1">
+        <v>0</v>
+      </c>
+      <c r="V82" s="1">
+        <v>0</v>
+      </c>
+      <c r="W82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S83" s="1">
+        <v>-3</v>
+      </c>
+      <c r="T83" s="1">
+        <v>-2</v>
+      </c>
+      <c r="U83" s="1">
+        <v>0</v>
+      </c>
+      <c r="V83" s="1">
+        <v>2</v>
+      </c>
+      <c r="W83" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W84" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V86" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N87" s="1">
+        <v>-3</v>
+      </c>
+      <c r="O87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P87" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>0</v>
+      </c>
+      <c r="R87" s="1">
+        <v>1</v>
+      </c>
+      <c r="S87" s="1">
+        <v>0</v>
+      </c>
+      <c r="T87" s="1">
+        <v>0</v>
+      </c>
+      <c r="U87" s="1">
+        <v>0</v>
+      </c>
+      <c r="V87" s="1">
+        <v>0</v>
+      </c>
+      <c r="W87" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y87" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S88" s="1">
+        <v>-2</v>
+      </c>
+      <c r="T88" s="1">
+        <v>-2</v>
+      </c>
+      <c r="U88" s="1">
+        <v>0</v>
+      </c>
+      <c r="V88" s="1">
+        <v>2</v>
+      </c>
+      <c r="W88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V89" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N92" s="1">
+        <v>-3</v>
+      </c>
+      <c r="O92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P92" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>0</v>
+      </c>
+      <c r="R92" s="1">
+        <v>1</v>
+      </c>
+      <c r="S92" s="1">
+        <v>0</v>
+      </c>
+      <c r="T92" s="1">
+        <v>0</v>
+      </c>
+      <c r="U92" s="1">
+        <v>0</v>
+      </c>
+      <c r="V92" s="1">
+        <v>2</v>
+      </c>
+      <c r="W92" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y92" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S93" s="1">
+        <v>-2</v>
+      </c>
+      <c r="T93" s="1">
+        <v>-2</v>
+      </c>
+      <c r="U93" s="1">
+        <v>0</v>
+      </c>
+      <c r="V93" s="1">
+        <v>0</v>
+      </c>
+      <c r="W93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U94" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="14:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="14:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N97" s="1">
+        <v>-3</v>
+      </c>
+      <c r="O97" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P97" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="1">
+        <v>0</v>
+      </c>
+      <c r="R97" s="1">
+        <v>0</v>
+      </c>
+      <c r="S97" s="1">
+        <v>0</v>
+      </c>
+      <c r="T97" s="1">
+        <v>0</v>
+      </c>
+      <c r="U97" s="1">
+        <v>1</v>
+      </c>
+      <c r="V97" s="1">
+        <v>2</v>
+      </c>
+      <c r="W97" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="14:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S98" s="1">
+        <v>-2</v>
+      </c>
+      <c r="T98" s="1">
+        <v>-2</v>
+      </c>
+      <c r="U98" s="1">
+        <v>0</v>
+      </c>
+      <c r="V98" s="1">
+        <v>0</v>
+      </c>
+      <c r="W98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="14:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V99" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>